<commit_message>
finished the contact information data
</commit_message>
<xml_diff>
--- a/Contact Information Data.xlsx
+++ b/Contact Information Data.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/AdamBrauns/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/AdamBrauns/Desktop/Git/OnlineGradeBook/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="420" yWindow="460" windowWidth="22020" windowHeight="19880" tabRatio="500"/>
+    <workbookView xWindow="40" yWindow="460" windowWidth="18360" windowHeight="14680" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="179">
   <si>
     <t>ID Number</t>
   </si>
@@ -92,30 +92,18 @@
     <t>RichieHanger@ums.edu</t>
   </si>
   <si>
-    <t>485 North Firthcliffe Circle</t>
-  </si>
-  <si>
     <t>682 South Tandy Gate</t>
   </si>
   <si>
-    <t>542 Old Tye Road</t>
-  </si>
-  <si>
     <t>482 West Mifflin Trail</t>
   </si>
   <si>
     <t>648 Star Point Road</t>
   </si>
   <si>
-    <t>846 Red Rum Pike Court</t>
-  </si>
-  <si>
     <t>565 West Howards Road</t>
   </si>
   <si>
-    <t>982 Northwest Praise Road</t>
-  </si>
-  <si>
     <t>MN</t>
   </si>
   <si>
@@ -137,12 +125,6 @@
     <t>548 Fox Creek Road</t>
   </si>
   <si>
-    <t>948 South Morning View Road</t>
-  </si>
-  <si>
-    <t>985 Hurley Parkway</t>
-  </si>
-  <si>
     <t>745 North Dolly Road</t>
   </si>
   <si>
@@ -150,6 +132,435 @@
   </si>
   <si>
     <t>336 Green Valley Road</t>
+  </si>
+  <si>
+    <t>JonasChauez@ums.edu</t>
+  </si>
+  <si>
+    <t>ElenorSetliff@ums.edu</t>
+  </si>
+  <si>
+    <t>TaylorServin@ums.edu</t>
+  </si>
+  <si>
+    <t>RossaMcanally@ums.edu</t>
+  </si>
+  <si>
+    <t>GrantPelayo@ums.edu</t>
+  </si>
+  <si>
+    <t>TamraAnderson@ums.edu</t>
+  </si>
+  <si>
+    <t>PhilipReamer@ums.edu</t>
+  </si>
+  <si>
+    <t>AlfredRhine@ums.edu</t>
+  </si>
+  <si>
+    <t>SueBratt@ums.edu</t>
+  </si>
+  <si>
+    <t>MartyLedford@ums.edu</t>
+  </si>
+  <si>
+    <t>TamaraGamble@ums.edu</t>
+  </si>
+  <si>
+    <t>DustinPhelps@ums.edu</t>
+  </si>
+  <si>
+    <t>ChristinaMiddleton@ums.edu</t>
+  </si>
+  <si>
+    <t>CaliPearson@ums.edu</t>
+  </si>
+  <si>
+    <t>RussellRowe@ums.edu</t>
+  </si>
+  <si>
+    <t>KyleRamos@ums.edu</t>
+  </si>
+  <si>
+    <t>JayleenMcConnell@ums.edu</t>
+  </si>
+  <si>
+    <t>MatthiasBruce@ums.edu</t>
+  </si>
+  <si>
+    <t>MarleyMooney@ums.edu</t>
+  </si>
+  <si>
+    <t>HollyNixon@ums.edu</t>
+  </si>
+  <si>
+    <t>NatalieWoods@ums.edu</t>
+  </si>
+  <si>
+    <t>JessieCain@ums.edu</t>
+  </si>
+  <si>
+    <t>KristenDuke@ums.edu</t>
+  </si>
+  <si>
+    <t>MelanieSoto@ums.edu</t>
+  </si>
+  <si>
+    <t>RyleeGoodman@ums.edu</t>
+  </si>
+  <si>
+    <t>SavannahVelez@ums.edu</t>
+  </si>
+  <si>
+    <t>DamionCooley@ums.edu</t>
+  </si>
+  <si>
+    <t>KellenKirby@ums.edu</t>
+  </si>
+  <si>
+    <t>DrakeRandolph@ums.edu</t>
+  </si>
+  <si>
+    <t>OwenDuran@ums.edu</t>
+  </si>
+  <si>
+    <t>PatrickGould@ums.edu</t>
+  </si>
+  <si>
+    <t>KyraFox@ums.edu</t>
+  </si>
+  <si>
+    <t>EthanWeber@ums.edu</t>
+  </si>
+  <si>
+    <t>MarieBoyd@ums.edu</t>
+  </si>
+  <si>
+    <t>AshlieKent@ums.edu</t>
+  </si>
+  <si>
+    <t>8132 Farland Avenue</t>
+  </si>
+  <si>
+    <t>2260 Bernardo Street</t>
+  </si>
+  <si>
+    <t>346 Benson Street</t>
+  </si>
+  <si>
+    <t>1294 Bolman Court</t>
+  </si>
+  <si>
+    <t>342 Hilcrest Avenue</t>
+  </si>
+  <si>
+    <t>342 Morgan Street</t>
+  </si>
+  <si>
+    <t>235 Rosemont Avenue</t>
+  </si>
+  <si>
+    <t>324 Short Street</t>
+  </si>
+  <si>
+    <t>3251 Browning Lane</t>
+  </si>
+  <si>
+    <t>919 Williams Avenue</t>
+  </si>
+  <si>
+    <t>8235 Tyler Avenue</t>
+  </si>
+  <si>
+    <t>9901 Caynor Circle</t>
+  </si>
+  <si>
+    <t>9389 James Martin Circle</t>
+  </si>
+  <si>
+    <t>2333 Chandler Drive</t>
+  </si>
+  <si>
+    <t>928 Ashmor Drive</t>
+  </si>
+  <si>
+    <t>9321 Tea Berry Lane</t>
+  </si>
+  <si>
+    <t>1298 Woodhill Avenue</t>
+  </si>
+  <si>
+    <t>1012 Neville Street</t>
+  </si>
+  <si>
+    <t>3320 Chipmunk Lane</t>
+  </si>
+  <si>
+    <t>2748 Cemetery Street</t>
+  </si>
+  <si>
+    <t>8772 Henery Street</t>
+  </si>
+  <si>
+    <t>1224 Renwick Drive</t>
+  </si>
+  <si>
+    <t>3421 University Drive</t>
+  </si>
+  <si>
+    <t>211 Clarksburg Road</t>
+  </si>
+  <si>
+    <t>1219 Maloy Court</t>
+  </si>
+  <si>
+    <t>4213 Rafe Lane</t>
+  </si>
+  <si>
+    <t>1229 Jacobs Street</t>
+  </si>
+  <si>
+    <t>442 Williams Road</t>
+  </si>
+  <si>
+    <t>5665 Benedum Drive</t>
+  </si>
+  <si>
+    <t>1254 Pinchelone Street</t>
+  </si>
+  <si>
+    <t>7668 Mesa Drive</t>
+  </si>
+  <si>
+    <t>5694 Pallet Street</t>
+  </si>
+  <si>
+    <t>1923 Saint Clair Street</t>
+  </si>
+  <si>
+    <t>8694 Neville Street</t>
+  </si>
+  <si>
+    <t>412 Crowford Drive</t>
+  </si>
+  <si>
+    <t>8912 Maloy Court</t>
+  </si>
+  <si>
+    <t>7643 Veltri Drive</t>
+  </si>
+  <si>
+    <t>1040 Coffman Alley</t>
+  </si>
+  <si>
+    <t>1002 Cross Street</t>
+  </si>
+  <si>
+    <t>5033 Dane Street</t>
+  </si>
+  <si>
+    <t>9809 Cherry Tree Drive</t>
+  </si>
+  <si>
+    <t>8701 Agriculture Lane</t>
+  </si>
+  <si>
+    <t>3098 Birch Street</t>
+  </si>
+  <si>
+    <t>806 Red Rum Pike Court</t>
+  </si>
+  <si>
+    <t>9042 Charter Street</t>
+  </si>
+  <si>
+    <t>540 Old Tye Road</t>
+  </si>
+  <si>
+    <t>905 Hurley Parkway</t>
+  </si>
+  <si>
+    <t>948 Morning View Road</t>
+  </si>
+  <si>
+    <t>982 Northwestern Road</t>
+  </si>
+  <si>
+    <t>485 Firthcliffe Circle</t>
+  </si>
+  <si>
+    <t>3195 Scheuvront Drive</t>
+  </si>
+  <si>
+    <t>9182 Saints Alley</t>
+  </si>
+  <si>
+    <t>1401 Whitetail Lane</t>
+  </si>
+  <si>
+    <t>9012 Kessla Way</t>
+  </si>
+  <si>
+    <t>2910 Simpson Square</t>
+  </si>
+  <si>
+    <t>5838 Terra Street</t>
+  </si>
+  <si>
+    <t>5810 Grant Street</t>
+  </si>
+  <si>
+    <t>7483 Pringle Drive</t>
+  </si>
+  <si>
+    <t>7010 Ingram Road</t>
+  </si>
+  <si>
+    <t>8219 Rainbow Road</t>
+  </si>
+  <si>
+    <t>8990 Valley Street</t>
+  </si>
+  <si>
+    <t>2931 Cambridge Drive</t>
+  </si>
+  <si>
+    <t>3285 Victoria Court</t>
+  </si>
+  <si>
+    <t>6749 Camden Street</t>
+  </si>
+  <si>
+    <t>9090 Oak Ridge Drive</t>
+  </si>
+  <si>
+    <t>8589 Oak Way</t>
+  </si>
+  <si>
+    <t>4827 Straford Park</t>
+  </si>
+  <si>
+    <t>3921 Langtown Road</t>
+  </si>
+  <si>
+    <t>7589 Moonlight Drive</t>
+  </si>
+  <si>
+    <t>7589 Copperhead Road</t>
+  </si>
+  <si>
+    <t>7548 Dale Avenue</t>
+  </si>
+  <si>
+    <t>6673 Blackwell Street</t>
+  </si>
+  <si>
+    <t>8680 Lords Way</t>
+  </si>
+  <si>
+    <t>1299 Williams Lane</t>
+  </si>
+  <si>
+    <t>9100 Oakmound Drive</t>
+  </si>
+  <si>
+    <t>1090 Green Street</t>
+  </si>
+  <si>
+    <t>1009 Conference Way</t>
+  </si>
+  <si>
+    <t>1920 Lake Forest Drive</t>
+  </si>
+  <si>
+    <t>3812 Hillcrest Circle</t>
+  </si>
+  <si>
+    <t>7318 Riverwood Drive</t>
+  </si>
+  <si>
+    <t>1394 Ridenour Street</t>
+  </si>
+  <si>
+    <t>1277 Bombardier Way</t>
+  </si>
+  <si>
+    <t>4198 Sunrise Road</t>
+  </si>
+  <si>
+    <t>5920 Hillview Street</t>
+  </si>
+  <si>
+    <t>6041 Clousson Road</t>
+  </si>
+  <si>
+    <t>6820 West Drive</t>
+  </si>
+  <si>
+    <t>6821 Mohlon Street</t>
+  </si>
+  <si>
+    <t>681 Garrett Street</t>
+  </si>
+  <si>
+    <t>468 Crim Lane</t>
+  </si>
+  <si>
+    <t>6829 Concord Street</t>
+  </si>
+  <si>
+    <t>689 Hardesty Street</t>
+  </si>
+  <si>
+    <t>6240 Long Street</t>
+  </si>
+  <si>
+    <t>MO</t>
+  </si>
+  <si>
+    <t>NE</t>
+  </si>
+  <si>
+    <t>SC</t>
+  </si>
+  <si>
+    <t>SD</t>
+  </si>
+  <si>
+    <t>TN</t>
+  </si>
+  <si>
+    <t>KY</t>
+  </si>
+  <si>
+    <t>AK</t>
+  </si>
+  <si>
+    <t>CA</t>
+  </si>
+  <si>
+    <t>NH</t>
+  </si>
+  <si>
+    <t>NY</t>
+  </si>
+  <si>
+    <t>WY</t>
+  </si>
+  <si>
+    <t>TX</t>
+  </si>
+  <si>
+    <t>GA</t>
+  </si>
+  <si>
+    <t>AR</t>
+  </si>
+  <si>
+    <t>CO</t>
+  </si>
+  <si>
+    <t>FL</t>
   </si>
 </sst>
 </file>
@@ -577,16 +988,16 @@
   <dimension ref="A1:G51"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="121" zoomScaleNormal="121" zoomScalePageLayoutView="121" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="J40" sqref="J40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="11.33203125" customWidth="1"/>
     <col min="2" max="2" width="14.33203125" customWidth="1"/>
-    <col min="3" max="3" width="24.83203125" customWidth="1"/>
-    <col min="4" max="4" width="27.1640625" customWidth="1"/>
-    <col min="5" max="5" width="26.83203125" customWidth="1"/>
+    <col min="3" max="3" width="26.5" customWidth="1"/>
+    <col min="4" max="4" width="24.33203125" customWidth="1"/>
+    <col min="5" max="5" width="22.6640625" customWidth="1"/>
     <col min="6" max="6" width="6.1640625" customWidth="1"/>
     <col min="7" max="7" width="10.1640625" customWidth="1"/>
   </cols>
@@ -625,13 +1036,13 @@
         <v>7</v>
       </c>
       <c r="D2" t="s">
-        <v>22</v>
+        <v>120</v>
       </c>
       <c r="E2" t="s">
-        <v>29</v>
+        <v>119</v>
       </c>
       <c r="F2" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="G2">
         <v>95685</v>
@@ -648,13 +1059,13 @@
         <v>8</v>
       </c>
       <c r="D3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E3" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="F3" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="G3">
         <v>46852</v>
@@ -671,13 +1082,13 @@
         <v>9</v>
       </c>
       <c r="D4" t="s">
-        <v>24</v>
+        <v>116</v>
       </c>
       <c r="E4" t="s">
-        <v>37</v>
+        <v>118</v>
       </c>
       <c r="F4" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="G4">
         <v>16856</v>
@@ -694,13 +1105,13 @@
         <v>10</v>
       </c>
       <c r="D5" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E5" t="s">
-        <v>38</v>
+        <v>117</v>
       </c>
       <c r="F5" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="G5">
         <v>78595</v>
@@ -717,13 +1128,13 @@
         <v>11</v>
       </c>
       <c r="D6" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E6" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="F6" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="G6">
         <v>20136</v>
@@ -740,13 +1151,13 @@
         <v>12</v>
       </c>
       <c r="D7" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="E7" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="F7" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="G7">
         <v>48487</v>
@@ -763,13 +1174,13 @@
         <v>13</v>
       </c>
       <c r="D8" t="s">
+        <v>114</v>
+      </c>
+      <c r="E8" t="s">
+        <v>35</v>
+      </c>
+      <c r="F8" t="s">
         <v>27</v>
-      </c>
-      <c r="E8" t="s">
-        <v>41</v>
-      </c>
-      <c r="F8" t="s">
-        <v>31</v>
       </c>
       <c r="G8">
         <v>98589</v>
@@ -785,6 +1196,18 @@
       <c r="C9" s="4" t="s">
         <v>14</v>
       </c>
+      <c r="D9" t="s">
+        <v>71</v>
+      </c>
+      <c r="E9" t="s">
+        <v>72</v>
+      </c>
+      <c r="F9" t="s">
+        <v>163</v>
+      </c>
+      <c r="G9">
+        <v>29385</v>
+      </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
@@ -796,6 +1219,18 @@
       <c r="C10" s="4" t="s">
         <v>15</v>
       </c>
+      <c r="D10" t="s">
+        <v>73</v>
+      </c>
+      <c r="E10" t="s">
+        <v>74</v>
+      </c>
+      <c r="F10" t="s">
+        <v>164</v>
+      </c>
+      <c r="G10">
+        <v>92834</v>
+      </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
@@ -807,6 +1242,18 @@
       <c r="C11" s="4" t="s">
         <v>16</v>
       </c>
+      <c r="D11" t="s">
+        <v>75</v>
+      </c>
+      <c r="E11" t="s">
+        <v>76</v>
+      </c>
+      <c r="F11" t="s">
+        <v>165</v>
+      </c>
+      <c r="G11">
+        <v>10204</v>
+      </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
@@ -818,6 +1265,18 @@
       <c r="C12" s="4" t="s">
         <v>17</v>
       </c>
+      <c r="D12" t="s">
+        <v>115</v>
+      </c>
+      <c r="E12" t="s">
+        <v>77</v>
+      </c>
+      <c r="F12" t="s">
+        <v>166</v>
+      </c>
+      <c r="G12">
+        <v>12523</v>
+      </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" s="2">
@@ -829,6 +1288,18 @@
       <c r="C13" s="4" t="s">
         <v>18</v>
       </c>
+      <c r="D13" t="s">
+        <v>78</v>
+      </c>
+      <c r="E13" t="s">
+        <v>79</v>
+      </c>
+      <c r="F13" t="s">
+        <v>167</v>
+      </c>
+      <c r="G13">
+        <v>58591</v>
+      </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
@@ -840,6 +1311,18 @@
       <c r="C14" s="4" t="s">
         <v>19</v>
       </c>
+      <c r="D14" t="s">
+        <v>80</v>
+      </c>
+      <c r="E14" t="s">
+        <v>81</v>
+      </c>
+      <c r="F14" t="s">
+        <v>168</v>
+      </c>
+      <c r="G14">
+        <v>10205</v>
+      </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" s="2">
@@ -851,6 +1334,18 @@
       <c r="C15" s="4" t="s">
         <v>20</v>
       </c>
+      <c r="D15" t="s">
+        <v>82</v>
+      </c>
+      <c r="E15" t="s">
+        <v>83</v>
+      </c>
+      <c r="F15" t="s">
+        <v>28</v>
+      </c>
+      <c r="G15">
+        <v>12035</v>
+      </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
@@ -859,183 +1354,825 @@
       <c r="B16">
         <v>9485200154</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C16" s="4" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D16" t="s">
+        <v>84</v>
+      </c>
+      <c r="E16" t="s">
+        <v>85</v>
+      </c>
+      <c r="F16" t="s">
+        <v>169</v>
+      </c>
+      <c r="G16">
+        <v>23405</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" s="2">
         <v>100015</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B17">
+        <v>3920684039</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="D17" t="s">
+        <v>113</v>
+      </c>
+      <c r="E17" t="s">
+        <v>86</v>
+      </c>
+      <c r="F17" t="s">
+        <v>27</v>
+      </c>
+      <c r="G17">
+        <v>10940</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <v>100016</v>
       </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B18">
+        <v>1928249205</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="D18" t="s">
+        <v>87</v>
+      </c>
+      <c r="E18" t="s">
+        <v>88</v>
+      </c>
+      <c r="F18" t="s">
+        <v>170</v>
+      </c>
+      <c r="G18">
+        <v>10200</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" s="2">
         <v>100017</v>
       </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B19">
+        <v>5298342492</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="D19" t="s">
+        <v>157</v>
+      </c>
+      <c r="E19" t="s">
+        <v>89</v>
+      </c>
+      <c r="F19" t="s">
+        <v>27</v>
+      </c>
+      <c r="G19">
+        <v>14912</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
         <v>100018</v>
       </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B20">
+        <v>2349323853</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="D20" t="s">
+        <v>90</v>
+      </c>
+      <c r="E20" t="s">
+        <v>91</v>
+      </c>
+      <c r="F20" t="s">
+        <v>28</v>
+      </c>
+      <c r="G20">
+        <v>95849</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" s="2">
         <v>100019</v>
       </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B21">
+        <v>9019384939</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="D21" t="s">
+        <v>112</v>
+      </c>
+      <c r="E21" t="s">
+        <v>92</v>
+      </c>
+      <c r="F21" t="s">
+        <v>163</v>
+      </c>
+      <c r="G21">
+        <v>38854</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
         <v>100020</v>
       </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B22">
+        <v>2854932923</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D22" t="s">
+        <v>93</v>
+      </c>
+      <c r="E22" t="s">
+        <v>94</v>
+      </c>
+      <c r="F22" t="s">
+        <v>164</v>
+      </c>
+      <c r="G22">
+        <v>34323</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" s="2">
         <v>100021</v>
       </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B23">
+        <v>1938295833</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D23" t="s">
+        <v>95</v>
+      </c>
+      <c r="E23" t="s">
+        <v>96</v>
+      </c>
+      <c r="F23" t="s">
+        <v>165</v>
+      </c>
+      <c r="G23">
+        <v>66203</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
         <v>100022</v>
       </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B24">
+        <v>3182983982</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="D24" t="s">
+        <v>111</v>
+      </c>
+      <c r="E24" t="s">
+        <v>97</v>
+      </c>
+      <c r="F24" t="s">
+        <v>171</v>
+      </c>
+      <c r="G24">
+        <v>91200</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" s="2">
         <v>100023</v>
       </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B25">
+        <v>2859283128</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="D25" t="s">
+        <v>98</v>
+      </c>
+      <c r="E25" t="s">
+        <v>99</v>
+      </c>
+      <c r="F25" t="s">
+        <v>172</v>
+      </c>
+      <c r="G25">
+        <v>14912</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
         <v>100024</v>
       </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B26">
+        <v>8583123812</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="D26" t="s">
+        <v>100</v>
+      </c>
+      <c r="E26" t="s">
+        <v>101</v>
+      </c>
+      <c r="F26" t="s">
+        <v>173</v>
+      </c>
+      <c r="G26">
+        <v>90800</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" s="2">
         <v>100025</v>
       </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B27">
+        <v>3582832923</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="D27" t="s">
+        <v>102</v>
+      </c>
+      <c r="E27" t="s">
+        <v>103</v>
+      </c>
+      <c r="F27" t="s">
+        <v>27</v>
+      </c>
+      <c r="G27">
+        <v>29400</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28" s="1">
         <v>100026</v>
       </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B28">
+        <v>3857548837</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="D28" t="s">
+        <v>104</v>
+      </c>
+      <c r="E28" t="s">
+        <v>105</v>
+      </c>
+      <c r="F28" t="s">
+        <v>28</v>
+      </c>
+      <c r="G28">
+        <v>73872</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29" s="2">
         <v>100027</v>
       </c>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B29">
+        <v>8929457343</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="D29" t="s">
+        <v>158</v>
+      </c>
+      <c r="E29" t="s">
+        <v>106</v>
+      </c>
+      <c r="F29" t="s">
+        <v>168</v>
+      </c>
+      <c r="G29">
+        <v>24859</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30" s="1">
         <v>100028</v>
       </c>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B30">
+        <v>2835863929</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="D30" t="s">
+        <v>107</v>
+      </c>
+      <c r="E30" t="s">
+        <v>161</v>
+      </c>
+      <c r="F30" t="s">
+        <v>169</v>
+      </c>
+      <c r="G30">
+        <v>89504</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31" s="2">
         <v>100029</v>
       </c>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B31">
+        <v>7718249932</v>
+      </c>
+      <c r="C31" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D31" t="s">
+        <v>108</v>
+      </c>
+      <c r="E31" t="s">
+        <v>109</v>
+      </c>
+      <c r="F31" t="s">
+        <v>27</v>
+      </c>
+      <c r="G31">
+        <v>21129</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32" s="1">
         <v>100030</v>
       </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B32">
+        <v>1288128994</v>
+      </c>
+      <c r="C32" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="D32" t="s">
+        <v>110</v>
+      </c>
+      <c r="E32" t="s">
+        <v>121</v>
+      </c>
+      <c r="F32" t="s">
+        <v>163</v>
+      </c>
+      <c r="G32">
+        <v>24502</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A33" s="2">
         <v>100031</v>
       </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B33">
+        <v>2342700124</v>
+      </c>
+      <c r="C33" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="D33" t="s">
+        <v>122</v>
+      </c>
+      <c r="E33" t="s">
+        <v>123</v>
+      </c>
+      <c r="F33" t="s">
+        <v>27</v>
+      </c>
+      <c r="G33">
+        <v>90654</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A34" s="1">
         <v>100032</v>
       </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B34">
+        <v>5834291230</v>
+      </c>
+      <c r="C34" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="D34" t="s">
+        <v>124</v>
+      </c>
+      <c r="E34" t="s">
+        <v>125</v>
+      </c>
+      <c r="F34" t="s">
+        <v>30</v>
+      </c>
+      <c r="G34">
+        <v>89302</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A35" s="2">
         <v>100033</v>
       </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B35">
+        <v>2385723812</v>
+      </c>
+      <c r="C35" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="D35" t="s">
+        <v>159</v>
+      </c>
+      <c r="E35" t="s">
+        <v>162</v>
+      </c>
+      <c r="F35" t="s">
+        <v>28</v>
+      </c>
+      <c r="G35">
+        <v>68842</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A36" s="1">
         <v>100034</v>
       </c>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B36">
+        <v>2375182394</v>
+      </c>
+      <c r="C36" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="D36" t="s">
+        <v>126</v>
+      </c>
+      <c r="E36" t="s">
+        <v>127</v>
+      </c>
+      <c r="F36" t="s">
+        <v>174</v>
+      </c>
+      <c r="G36">
+        <v>52049</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A37" s="2">
         <v>100035</v>
       </c>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B37">
+        <v>6737231824</v>
+      </c>
+      <c r="C37" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="D37" t="s">
+        <v>128</v>
+      </c>
+      <c r="E37" t="s">
+        <v>129</v>
+      </c>
+      <c r="F37" t="s">
+        <v>27</v>
+      </c>
+      <c r="G37">
+        <v>77873</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A38" s="1">
         <v>100036</v>
       </c>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B38">
+        <v>5868329102</v>
+      </c>
+      <c r="C38" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="D38" t="s">
+        <v>130</v>
+      </c>
+      <c r="E38" t="s">
+        <v>131</v>
+      </c>
+      <c r="F38" t="s">
+        <v>175</v>
+      </c>
+      <c r="G38">
+        <v>85490</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A39" s="2">
         <v>100037</v>
       </c>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B39">
+        <v>3858329128</v>
+      </c>
+      <c r="C39" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="D39" t="s">
+        <v>132</v>
+      </c>
+      <c r="E39" t="s">
+        <v>133</v>
+      </c>
+      <c r="F39" t="s">
+        <v>27</v>
+      </c>
+      <c r="G39">
+        <v>90339</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A40" s="1">
         <v>100038</v>
       </c>
-    </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B40">
+        <v>7538238343</v>
+      </c>
+      <c r="C40" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="D40" t="s">
+        <v>134</v>
+      </c>
+      <c r="E40" t="s">
+        <v>135</v>
+      </c>
+      <c r="F40" t="s">
+        <v>28</v>
+      </c>
+      <c r="G40">
+        <v>29004</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A41" s="2">
         <v>100039</v>
       </c>
-    </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B41">
+        <v>8912875884</v>
+      </c>
+      <c r="C41" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="D41" t="s">
+        <v>136</v>
+      </c>
+      <c r="E41" t="s">
+        <v>137</v>
+      </c>
+      <c r="F41" t="s">
+        <v>164</v>
+      </c>
+      <c r="G41">
+        <v>37583</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A42" s="1">
         <v>100040</v>
       </c>
-    </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B42">
+        <v>1299211932</v>
+      </c>
+      <c r="C42" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="D42" t="s">
+        <v>138</v>
+      </c>
+      <c r="E42" t="s">
+        <v>139</v>
+      </c>
+      <c r="F42" t="s">
+        <v>163</v>
+      </c>
+      <c r="G42">
+        <v>82994</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A43" s="2">
         <v>100041</v>
       </c>
-    </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B43">
+        <v>4032941901</v>
+      </c>
+      <c r="C43" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="D43" t="s">
+        <v>140</v>
+      </c>
+      <c r="E43" t="s">
+        <v>141</v>
+      </c>
+      <c r="F43" t="s">
+        <v>27</v>
+      </c>
+      <c r="G43">
+        <v>82875</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A44" s="1">
         <v>100042</v>
       </c>
-    </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B44">
+        <v>5939823932</v>
+      </c>
+      <c r="C44" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="D44" t="s">
+        <v>142</v>
+      </c>
+      <c r="E44" t="s">
+        <v>143</v>
+      </c>
+      <c r="F44" t="s">
+        <v>168</v>
+      </c>
+      <c r="G44">
+        <v>27478</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A45" s="2">
         <v>100043</v>
       </c>
-    </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B45">
+        <v>8283983052</v>
+      </c>
+      <c r="C45" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="D45" t="s">
+        <v>144</v>
+      </c>
+      <c r="E45" t="s">
+        <v>145</v>
+      </c>
+      <c r="F45" t="s">
+        <v>169</v>
+      </c>
+      <c r="G45">
+        <v>19924</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A46" s="1">
         <v>100044</v>
       </c>
-    </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B46">
+        <v>7378399913</v>
+      </c>
+      <c r="C46" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="D46" t="s">
+        <v>146</v>
+      </c>
+      <c r="E46" t="s">
+        <v>151</v>
+      </c>
+      <c r="F46" t="s">
+        <v>28</v>
+      </c>
+      <c r="G46">
+        <v>74592</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A47" s="2">
         <v>100045</v>
       </c>
-    </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B47">
+        <v>2905948848</v>
+      </c>
+      <c r="C47" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="D47" t="s">
+        <v>160</v>
+      </c>
+      <c r="E47" t="s">
+        <v>152</v>
+      </c>
+      <c r="F47" t="s">
+        <v>27</v>
+      </c>
+      <c r="G47">
+        <v>85749</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A48" s="1">
         <v>100046</v>
       </c>
-    </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B48">
+        <v>3829191912</v>
+      </c>
+      <c r="C48" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="D48" t="s">
+        <v>147</v>
+      </c>
+      <c r="E48" t="s">
+        <v>153</v>
+      </c>
+      <c r="F48" t="s">
+        <v>27</v>
+      </c>
+      <c r="G48">
+        <v>59288</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A49" s="2">
         <v>100047</v>
       </c>
-    </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B49">
+        <v>4848234222</v>
+      </c>
+      <c r="C49" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="D49" t="s">
+        <v>148</v>
+      </c>
+      <c r="E49" t="s">
+        <v>154</v>
+      </c>
+      <c r="F49" t="s">
+        <v>176</v>
+      </c>
+      <c r="G49">
+        <v>57492</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A50" s="1">
         <v>100048</v>
       </c>
-    </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B50">
+        <v>9812758829</v>
+      </c>
+      <c r="C50" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="D50" t="s">
+        <v>149</v>
+      </c>
+      <c r="E50" t="s">
+        <v>155</v>
+      </c>
+      <c r="F50" t="s">
+        <v>177</v>
+      </c>
+      <c r="G50">
+        <v>49835</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A51" s="3">
         <v>100049</v>
+      </c>
+      <c r="B51">
+        <v>9283484748</v>
+      </c>
+      <c r="C51" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="D51" t="s">
+        <v>150</v>
+      </c>
+      <c r="E51" t="s">
+        <v>156</v>
+      </c>
+      <c r="F51" t="s">
+        <v>178</v>
+      </c>
+      <c r="G51">
+        <v>87355</v>
       </c>
     </row>
   </sheetData>
@@ -1054,10 +2191,46 @@
     <hyperlink ref="C13" r:id="rId12"/>
     <hyperlink ref="C14" r:id="rId13"/>
     <hyperlink ref="C15" r:id="rId14"/>
+    <hyperlink ref="C17" r:id="rId15"/>
+    <hyperlink ref="C18" r:id="rId16"/>
+    <hyperlink ref="C19" r:id="rId17"/>
+    <hyperlink ref="C16" r:id="rId18"/>
+    <hyperlink ref="C20" r:id="rId19"/>
+    <hyperlink ref="C21" r:id="rId20"/>
+    <hyperlink ref="C22" r:id="rId21"/>
+    <hyperlink ref="C23" r:id="rId22"/>
+    <hyperlink ref="C24" r:id="rId23"/>
+    <hyperlink ref="C25" r:id="rId24"/>
+    <hyperlink ref="C26" r:id="rId25"/>
+    <hyperlink ref="C27" r:id="rId26"/>
+    <hyperlink ref="C28" r:id="rId27"/>
+    <hyperlink ref="C29" r:id="rId28"/>
+    <hyperlink ref="C30" r:id="rId29"/>
+    <hyperlink ref="C31" r:id="rId30"/>
+    <hyperlink ref="C32" r:id="rId31"/>
+    <hyperlink ref="C33" r:id="rId32"/>
+    <hyperlink ref="C34" r:id="rId33"/>
+    <hyperlink ref="C35" r:id="rId34"/>
+    <hyperlink ref="C36" r:id="rId35"/>
+    <hyperlink ref="C37" r:id="rId36"/>
+    <hyperlink ref="C38" r:id="rId37"/>
+    <hyperlink ref="C39" r:id="rId38"/>
+    <hyperlink ref="C40" r:id="rId39"/>
+    <hyperlink ref="C41" r:id="rId40"/>
+    <hyperlink ref="C42" r:id="rId41"/>
+    <hyperlink ref="C43" r:id="rId42"/>
+    <hyperlink ref="C44" r:id="rId43"/>
+    <hyperlink ref="C45" r:id="rId44"/>
+    <hyperlink ref="C46" r:id="rId45"/>
+    <hyperlink ref="C47" r:id="rId46"/>
+    <hyperlink ref="C48" r:id="rId47"/>
+    <hyperlink ref="C49" r:id="rId48"/>
+    <hyperlink ref="C50" r:id="rId49"/>
+    <hyperlink ref="C51" r:id="rId50"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
-    <tablePart r:id="rId15"/>
+    <tablePart r:id="rId51"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>